<commit_message>
phần uyên và quỳnh đã chỉnh sửa xong
</commit_message>
<xml_diff>
--- a/KH_HUE_T08_DatabaseDesign_v3.0.xlsx
+++ b/KH_HUE_T08_DatabaseDesign_v3.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="74">
   <si>
     <t>Tên cột</t>
     <phoneticPr fontId="0"/>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2133,7 @@
         <v>48</v>
       </c>
       <c r="E78" s="2">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="5"/>
@@ -2158,11 +2161,9 @@
         <v>54</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E79" s="2">
-        <v>50</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>

</xml_diff>